<commit_message>
Add ContractNumber and ContractDate
</commit_message>
<xml_diff>
--- a/resources/invoice_template_empl.xlsx
+++ b/resources/invoice_template_empl.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>INVOICE</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>Invoice Number: %D%</t>
+  </si>
+  <si>
+    <t>Contract Number: %S%</t>
+  </si>
+  <si>
+    <t>Contract Date: %S%</t>
   </si>
 </sst>
 </file>
@@ -212,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -224,20 +230,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -245,10 +238,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -257,6 +258,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM1000"/>
+  <dimension ref="A1:AM1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="U37" sqref="U37:AM37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38:AM38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -641,8 +648,9 @@
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="AM2" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -682,9 +690,7 @@
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
-      <c r="AM3" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="AM3" s="1"/>
     </row>
     <row r="4" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -724,7 +730,9 @@
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
-      <c r="AM4" s="1"/>
+      <c r="AM4" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -765,10 +773,10 @@
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
       <c r="AM5" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -807,13 +815,11 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AM6" s="3" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>2</v>
-      </c>
+    <row r="7" spans="1:39" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -850,507 +856,508 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
-      <c r="AL7" s="1"/>
-      <c r="AM7" s="1"/>
+      <c r="AM7" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+    </row>
+    <row r="9" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
-      <c r="AG8" s="5"/>
-      <c r="AH8" s="5"/>
-      <c r="AI8" s="5"/>
-      <c r="AJ8" s="5"/>
-      <c r="AK8" s="5"/>
-      <c r="AL8" s="5"/>
-      <c r="AM8" s="5"/>
-    </row>
-    <row r="9" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="5"/>
-      <c r="AB9" s="5"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
-      <c r="AE9" s="5"/>
-      <c r="AF9" s="5"/>
-      <c r="AG9" s="5"/>
-      <c r="AH9" s="5"/>
-      <c r="AI9" s="5"/>
-      <c r="AJ9" s="5"/>
-      <c r="AK9" s="5"/>
-      <c r="AL9" s="5"/>
-      <c r="AM9" s="5"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="5"/>
-      <c r="AH10" s="5"/>
-      <c r="AI10" s="5"/>
-      <c r="AJ10" s="5"/>
-      <c r="AK10" s="5"/>
-      <c r="AL10" s="5"/>
-      <c r="AM10" s="5"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
     </row>
     <row r="11" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="5"/>
-      <c r="AC11" s="5"/>
-      <c r="AD11" s="5"/>
-      <c r="AE11" s="5"/>
-      <c r="AF11" s="5"/>
-      <c r="AG11" s="5"/>
-      <c r="AH11" s="5"/>
-      <c r="AI11" s="5"/>
-      <c r="AJ11" s="5"/>
-      <c r="AK11" s="5"/>
-      <c r="AL11" s="5"/>
-      <c r="AM11" s="5"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
     </row>
     <row r="12" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="5"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="5"/>
-      <c r="AE12" s="5"/>
-      <c r="AF12" s="5"/>
-      <c r="AG12" s="5"/>
-      <c r="AH12" s="5"/>
-      <c r="AI12" s="5"/>
-      <c r="AJ12" s="5"/>
-      <c r="AK12" s="5"/>
-      <c r="AL12" s="5"/>
-      <c r="AM12" s="5"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
     </row>
     <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="5"/>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="5"/>
-      <c r="AE13" s="5"/>
-      <c r="AF13" s="5"/>
-      <c r="AG13" s="5"/>
-      <c r="AH13" s="5"/>
-      <c r="AI13" s="5"/>
-      <c r="AJ13" s="5"/>
-      <c r="AK13" s="5"/>
-      <c r="AL13" s="5"/>
-      <c r="AM13" s="5"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+      <c r="AJ13" s="9"/>
+      <c r="AK13" s="9"/>
+      <c r="AL13" s="9"/>
+      <c r="AM13" s="9"/>
     </row>
     <row r="14" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="5"/>
-      <c r="AB14" s="5"/>
-      <c r="AC14" s="5"/>
-      <c r="AD14" s="5"/>
-      <c r="AE14" s="5"/>
-      <c r="AF14" s="5"/>
-      <c r="AG14" s="5"/>
-      <c r="AH14" s="5"/>
-      <c r="AI14" s="5"/>
-      <c r="AJ14" s="5"/>
-      <c r="AK14" s="5"/>
-      <c r="AL14" s="5"/>
-      <c r="AM14" s="5"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="9"/>
+      <c r="AJ14" s="9"/>
+      <c r="AK14" s="9"/>
+      <c r="AL14" s="9"/>
+      <c r="AM14" s="9"/>
     </row>
     <row r="15" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
-      <c r="AA15" s="5"/>
-      <c r="AB15" s="5"/>
-      <c r="AC15" s="5"/>
-      <c r="AD15" s="5"/>
-      <c r="AE15" s="5"/>
-      <c r="AF15" s="5"/>
-      <c r="AG15" s="5"/>
-      <c r="AH15" s="5"/>
-      <c r="AI15" s="5"/>
-      <c r="AJ15" s="5"/>
-      <c r="AK15" s="5"/>
-      <c r="AL15" s="5"/>
-      <c r="AM15" s="5"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="9"/>
+      <c r="AK15" s="9"/>
+      <c r="AL15" s="9"/>
+      <c r="AM15" s="9"/>
     </row>
     <row r="16" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="5"/>
-      <c r="Y16" s="5"/>
-      <c r="Z16" s="5"/>
-      <c r="AA16" s="5"/>
-      <c r="AB16" s="5"/>
-      <c r="AC16" s="5"/>
-      <c r="AD16" s="5"/>
-      <c r="AE16" s="5"/>
-      <c r="AF16" s="5"/>
-      <c r="AG16" s="5"/>
-      <c r="AH16" s="5"/>
-      <c r="AI16" s="5"/>
-      <c r="AJ16" s="5"/>
-      <c r="AK16" s="5"/>
-      <c r="AL16" s="5"/>
-      <c r="AM16" s="5"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
+      <c r="AJ16" s="9"/>
+      <c r="AK16" s="9"/>
+      <c r="AL16" s="9"/>
+      <c r="AM16" s="9"/>
     </row>
     <row r="17" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
-      <c r="AA17" s="5"/>
-      <c r="AB17" s="5"/>
-      <c r="AC17" s="5"/>
-      <c r="AD17" s="5"/>
-      <c r="AE17" s="5"/>
-      <c r="AF17" s="5"/>
-      <c r="AG17" s="5"/>
-      <c r="AH17" s="5"/>
-      <c r="AI17" s="5"/>
-      <c r="AJ17" s="5"/>
-      <c r="AK17" s="5"/>
-      <c r="AL17" s="5"/>
-      <c r="AM17" s="5"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="9"/>
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="9"/>
+      <c r="AL17" s="9"/>
+      <c r="AM17" s="9"/>
     </row>
     <row r="18" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
-      <c r="Y18" s="5"/>
-      <c r="Z18" s="5"/>
-      <c r="AA18" s="5"/>
-      <c r="AB18" s="5"/>
-      <c r="AC18" s="5"/>
-      <c r="AD18" s="5"/>
-      <c r="AE18" s="5"/>
-      <c r="AF18" s="5"/>
-      <c r="AG18" s="5"/>
-      <c r="AH18" s="5"/>
-      <c r="AI18" s="5"/>
-      <c r="AJ18" s="5"/>
-      <c r="AK18" s="5"/>
-      <c r="AL18" s="5"/>
-      <c r="AM18" s="5"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="9"/>
+      <c r="AI18" s="9"/>
+      <c r="AJ18" s="9"/>
+      <c r="AK18" s="9"/>
+      <c r="AL18" s="9"/>
+      <c r="AM18" s="9"/>
     </row>
     <row r="19" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-      <c r="AE19" s="1"/>
-      <c r="AF19" s="1"/>
-      <c r="AG19" s="1"/>
-      <c r="AH19" s="1"/>
-      <c r="AI19" s="1"/>
-      <c r="AJ19" s="1"/>
-      <c r="AK19" s="1"/>
-      <c r="AL19" s="1"/>
-      <c r="AM19" s="1"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="9"/>
+      <c r="AL19" s="9"/>
+      <c r="AM19" s="9"/>
     </row>
     <row r="20" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1391,482 +1398,491 @@
       <c r="AM20" s="1"/>
     </row>
     <row r="21" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="1"/>
+      <c r="AL21" s="1"/>
+      <c r="AM21" s="1"/>
+    </row>
+    <row r="22" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="13"/>
-      <c r="Z21" s="13"/>
-      <c r="AA21" s="13"/>
-      <c r="AB21" s="13"/>
-      <c r="AC21" s="13"/>
-      <c r="AD21" s="13"/>
-      <c r="AE21" s="13"/>
-      <c r="AF21" s="13"/>
-      <c r="AG21" s="13"/>
-      <c r="AH21" s="13"/>
-      <c r="AI21" s="13"/>
-      <c r="AJ21" s="13"/>
-      <c r="AK21" s="13"/>
-      <c r="AL21" s="13"/>
-      <c r="AM21" s="13"/>
-    </row>
-    <row r="22" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
-      <c r="W22" s="13"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
-      <c r="Z22" s="13"/>
-      <c r="AA22" s="13"/>
-      <c r="AB22" s="13"/>
-      <c r="AC22" s="13"/>
-      <c r="AD22" s="13"/>
-      <c r="AE22" s="13"/>
-      <c r="AF22" s="13"/>
-      <c r="AG22" s="13"/>
-      <c r="AH22" s="13"/>
-      <c r="AI22" s="13"/>
-      <c r="AJ22" s="13"/>
-      <c r="AK22" s="13"/>
-      <c r="AL22" s="13"/>
-      <c r="AM22" s="13"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="8"/>
+      <c r="AC22" s="8"/>
+      <c r="AD22" s="8"/>
+      <c r="AE22" s="8"/>
+      <c r="AF22" s="8"/>
+      <c r="AG22" s="8"/>
+      <c r="AH22" s="8"/>
+      <c r="AI22" s="8"/>
+      <c r="AJ22" s="8"/>
+      <c r="AK22" s="8"/>
+      <c r="AL22" s="8"/>
+      <c r="AM22" s="8"/>
     </row>
     <row r="23" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
-      <c r="W23" s="13"/>
-      <c r="X23" s="13"/>
-      <c r="Y23" s="13"/>
-      <c r="Z23" s="13"/>
-      <c r="AA23" s="13"/>
-      <c r="AB23" s="13"/>
-      <c r="AC23" s="13"/>
-      <c r="AD23" s="13"/>
-      <c r="AE23" s="13"/>
-      <c r="AF23" s="13"/>
-      <c r="AG23" s="13"/>
-      <c r="AH23" s="13"/>
-      <c r="AI23" s="13"/>
-      <c r="AJ23" s="13"/>
-      <c r="AK23" s="13"/>
-      <c r="AL23" s="13"/>
-      <c r="AM23" s="13"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+      <c r="AC23" s="8"/>
+      <c r="AD23" s="8"/>
+      <c r="AE23" s="8"/>
+      <c r="AF23" s="8"/>
+      <c r="AG23" s="8"/>
+      <c r="AH23" s="8"/>
+      <c r="AI23" s="8"/>
+      <c r="AJ23" s="8"/>
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="8"/>
+      <c r="AM23" s="8"/>
     </row>
     <row r="24" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="13"/>
-      <c r="W24" s="13"/>
-      <c r="X24" s="13"/>
-      <c r="Y24" s="13"/>
-      <c r="Z24" s="13"/>
-      <c r="AA24" s="13"/>
-      <c r="AB24" s="13"/>
-      <c r="AC24" s="13"/>
-      <c r="AD24" s="13"/>
-      <c r="AE24" s="13"/>
-      <c r="AF24" s="13"/>
-      <c r="AG24" s="13"/>
-      <c r="AH24" s="13"/>
-      <c r="AI24" s="13"/>
-      <c r="AJ24" s="13"/>
-      <c r="AK24" s="13"/>
-      <c r="AL24" s="13"/>
-      <c r="AM24" s="13"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="8"/>
+      <c r="AB24" s="8"/>
+      <c r="AC24" s="8"/>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="8"/>
+      <c r="AF24" s="8"/>
+      <c r="AG24" s="8"/>
+      <c r="AH24" s="8"/>
+      <c r="AI24" s="8"/>
+      <c r="AJ24" s="8"/>
+      <c r="AK24" s="8"/>
+      <c r="AL24" s="8"/>
+      <c r="AM24" s="8"/>
     </row>
     <row r="25" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="13"/>
-      <c r="W25" s="13"/>
-      <c r="X25" s="13"/>
-      <c r="Y25" s="13"/>
-      <c r="Z25" s="13"/>
-      <c r="AA25" s="13"/>
-      <c r="AB25" s="13"/>
-      <c r="AC25" s="13"/>
-      <c r="AD25" s="13"/>
-      <c r="AE25" s="13"/>
-      <c r="AF25" s="13"/>
-      <c r="AG25" s="13"/>
-      <c r="AH25" s="13"/>
-      <c r="AI25" s="13"/>
-      <c r="AJ25" s="13"/>
-      <c r="AK25" s="13"/>
-      <c r="AL25" s="13"/>
-      <c r="AM25" s="13"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="8"/>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="8"/>
+      <c r="AB25" s="8"/>
+      <c r="AC25" s="8"/>
+      <c r="AD25" s="8"/>
+      <c r="AE25" s="8"/>
+      <c r="AF25" s="8"/>
+      <c r="AG25" s="8"/>
+      <c r="AH25" s="8"/>
+      <c r="AI25" s="8"/>
+      <c r="AJ25" s="8"/>
+      <c r="AK25" s="8"/>
+      <c r="AL25" s="8"/>
+      <c r="AM25" s="8"/>
     </row>
     <row r="26" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
-      <c r="AA26" s="1"/>
-      <c r="AB26" s="1"/>
-      <c r="AC26" s="1"/>
-      <c r="AD26" s="1"/>
-      <c r="AE26" s="1"/>
-      <c r="AF26" s="1"/>
-      <c r="AG26" s="1"/>
-      <c r="AH26" s="1"/>
-      <c r="AI26" s="1"/>
-      <c r="AJ26" s="1"/>
-      <c r="AK26" s="1"/>
-      <c r="AL26" s="1"/>
-      <c r="AM26" s="1"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="8"/>
+      <c r="AB26" s="8"/>
+      <c r="AC26" s="8"/>
+      <c r="AD26" s="8"/>
+      <c r="AE26" s="8"/>
+      <c r="AF26" s="8"/>
+      <c r="AG26" s="8"/>
+      <c r="AH26" s="8"/>
+      <c r="AI26" s="8"/>
+      <c r="AJ26" s="8"/>
+      <c r="AK26" s="8"/>
+      <c r="AL26" s="8"/>
+      <c r="AM26" s="8"/>
     </row>
     <row r="27" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="1"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+      <c r="AL27" s="1"/>
+      <c r="AM27" s="1"/>
+    </row>
+    <row r="28" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="10" t="s">
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-      <c r="V27" s="8"/>
-      <c r="W27" s="10" t="s">
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="14"/>
+      <c r="W28" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27" s="10" t="s">
+      <c r="X28" s="13"/>
+      <c r="Y28" s="14"/>
+      <c r="Z28" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AA27" s="7"/>
-      <c r="AB27" s="7"/>
-      <c r="AC27" s="7"/>
-      <c r="AD27" s="8"/>
-      <c r="AE27" s="10" t="s">
+      <c r="AA28" s="13"/>
+      <c r="AB28" s="13"/>
+      <c r="AC28" s="13"/>
+      <c r="AD28" s="14"/>
+      <c r="AE28" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AF27" s="7"/>
-      <c r="AG27" s="8"/>
-      <c r="AH27" s="10" t="s">
+      <c r="AF28" s="13"/>
+      <c r="AG28" s="14"/>
+      <c r="AH28" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="AI27" s="7"/>
-      <c r="AJ27" s="7"/>
-      <c r="AK27" s="7"/>
-      <c r="AL27" s="7"/>
-      <c r="AM27" s="8"/>
-    </row>
-    <row r="28" spans="1:39" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="AI28" s="13"/>
+      <c r="AJ28" s="13"/>
+      <c r="AK28" s="13"/>
+      <c r="AL28" s="13"/>
+      <c r="AM28" s="14"/>
+    </row>
+    <row r="29" spans="1:39" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="19">
         <v>1</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="6" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="9" t="s">
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="14"/>
+      <c r="W29" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="X28" s="7"/>
-      <c r="Y28" s="8"/>
-      <c r="Z28" s="18" t="s">
+      <c r="X29" s="13"/>
+      <c r="Y29" s="14"/>
+      <c r="Z29" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="AA28" s="7"/>
-      <c r="AB28" s="7"/>
-      <c r="AC28" s="7"/>
-      <c r="AD28" s="8"/>
-      <c r="AE28" s="18" t="s">
+      <c r="AA29" s="13"/>
+      <c r="AB29" s="13"/>
+      <c r="AC29" s="13"/>
+      <c r="AD29" s="14"/>
+      <c r="AE29" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="AF28" s="7"/>
-      <c r="AG28" s="8"/>
-      <c r="AH28" s="18" t="s">
+      <c r="AF29" s="13"/>
+      <c r="AG29" s="14"/>
+      <c r="AH29" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="AI28" s="7"/>
-      <c r="AJ28" s="7"/>
-      <c r="AK28" s="7"/>
-      <c r="AL28" s="7"/>
-      <c r="AM28" s="8"/>
-    </row>
-    <row r="29" spans="1:39" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="AI29" s="13"/>
+      <c r="AJ29" s="13"/>
+      <c r="AK29" s="13"/>
+      <c r="AL29" s="13"/>
+      <c r="AM29" s="14"/>
+    </row>
+    <row r="30" spans="1:39" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="7"/>
-      <c r="W29" s="7"/>
-      <c r="X29" s="7"/>
-      <c r="Y29" s="7"/>
-      <c r="Z29" s="7"/>
-      <c r="AA29" s="7"/>
-      <c r="AB29" s="7"/>
-      <c r="AC29" s="7"/>
-      <c r="AD29" s="7"/>
-      <c r="AE29" s="7"/>
-      <c r="AF29" s="7"/>
-      <c r="AG29" s="8"/>
-      <c r="AH29" s="16" t="s">
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
+      <c r="Z30" s="13"/>
+      <c r="AA30" s="13"/>
+      <c r="AB30" s="13"/>
+      <c r="AC30" s="13"/>
+      <c r="AD30" s="13"/>
+      <c r="AE30" s="13"/>
+      <c r="AF30" s="13"/>
+      <c r="AG30" s="14"/>
+      <c r="AH30" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AI29" s="7"/>
-      <c r="AJ29" s="7"/>
-      <c r="AK29" s="7"/>
-      <c r="AL29" s="7"/>
-      <c r="AM29" s="8"/>
-    </row>
-    <row r="30" spans="1:39" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="AI30" s="13"/>
+      <c r="AJ30" s="13"/>
+      <c r="AK30" s="13"/>
+      <c r="AL30" s="13"/>
+      <c r="AM30" s="14"/>
+    </row>
+    <row r="31" spans="1:39" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
-      <c r="V30" s="7"/>
-      <c r="W30" s="7"/>
-      <c r="X30" s="7"/>
-      <c r="Y30" s="7"/>
-      <c r="Z30" s="7"/>
-      <c r="AA30" s="7"/>
-      <c r="AB30" s="7"/>
-      <c r="AC30" s="7"/>
-      <c r="AD30" s="7"/>
-      <c r="AE30" s="7"/>
-      <c r="AF30" s="7"/>
-      <c r="AG30" s="8"/>
-      <c r="AH30" s="16" t="s">
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="13"/>
+      <c r="AA31" s="13"/>
+      <c r="AB31" s="13"/>
+      <c r="AC31" s="13"/>
+      <c r="AD31" s="13"/>
+      <c r="AE31" s="13"/>
+      <c r="AF31" s="13"/>
+      <c r="AG31" s="14"/>
+      <c r="AH31" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AI30" s="7"/>
-      <c r="AJ30" s="7"/>
-      <c r="AK30" s="7"/>
-      <c r="AL30" s="7"/>
-      <c r="AM30" s="8"/>
-    </row>
-    <row r="31" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
-      <c r="AA31" s="1"/>
-      <c r="AB31" s="1"/>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="1"/>
-      <c r="AE31" s="1"/>
-      <c r="AF31" s="1"/>
-      <c r="AG31" s="1"/>
-      <c r="AH31" s="1"/>
-      <c r="AI31" s="1"/>
-      <c r="AJ31" s="1"/>
-      <c r="AK31" s="1"/>
-      <c r="AL31" s="1"/>
-      <c r="AM31" s="1"/>
+      <c r="AI31" s="13"/>
+      <c r="AJ31" s="13"/>
+      <c r="AK31" s="13"/>
+      <c r="AL31" s="13"/>
+      <c r="AM31" s="14"/>
     </row>
     <row r="32" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H32" s="1"/>
@@ -1900,9 +1916,7 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
       <c r="AL32" s="1"/>
-      <c r="AM32" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="AM32" s="1"/>
     </row>
     <row r="33" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H33" s="1"/>
@@ -1936,18 +1950,11 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
       <c r="AL33" s="1"/>
-      <c r="AM33" s="3" t="s">
-        <v>17</v>
+      <c r="AM33" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1979,7 +1986,9 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
       <c r="AL34" s="1"/>
-      <c r="AM34" s="1"/>
+      <c r="AM34" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="35" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
@@ -2084,25 +2093,25 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
-      <c r="U37" s="11"/>
-      <c r="V37" s="12"/>
-      <c r="W37" s="12"/>
-      <c r="X37" s="12"/>
-      <c r="Y37" s="12"/>
-      <c r="Z37" s="12"/>
-      <c r="AA37" s="12"/>
-      <c r="AB37" s="12"/>
-      <c r="AC37" s="12"/>
-      <c r="AD37" s="12"/>
-      <c r="AE37" s="12"/>
-      <c r="AF37" s="12"/>
-      <c r="AG37" s="12"/>
-      <c r="AH37" s="12"/>
-      <c r="AI37" s="12"/>
-      <c r="AJ37" s="12"/>
-      <c r="AK37" s="12"/>
-      <c r="AL37" s="12"/>
-      <c r="AM37" s="12"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
+      <c r="AF37" s="1"/>
+      <c r="AG37" s="1"/>
+      <c r="AH37" s="1"/>
+      <c r="AI37" s="1"/>
+      <c r="AJ37" s="1"/>
+      <c r="AK37" s="1"/>
+      <c r="AL37" s="1"/>
+      <c r="AM37" s="1"/>
     </row>
     <row r="38" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
@@ -2125,27 +2134,25 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
-      <c r="U38" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="V38" s="15"/>
-      <c r="W38" s="15"/>
-      <c r="X38" s="15"/>
-      <c r="Y38" s="15"/>
-      <c r="Z38" s="15"/>
-      <c r="AA38" s="15"/>
-      <c r="AB38" s="15"/>
-      <c r="AC38" s="15"/>
-      <c r="AD38" s="15"/>
-      <c r="AE38" s="15"/>
-      <c r="AF38" s="15"/>
-      <c r="AG38" s="15"/>
-      <c r="AH38" s="15"/>
-      <c r="AI38" s="15"/>
-      <c r="AJ38" s="15"/>
-      <c r="AK38" s="15"/>
-      <c r="AL38" s="15"/>
-      <c r="AM38" s="15"/>
+      <c r="U38" s="6"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="7"/>
+      <c r="AG38" s="7"/>
+      <c r="AH38" s="7"/>
+      <c r="AI38" s="7"/>
+      <c r="AJ38" s="7"/>
+      <c r="AK38" s="7"/>
+      <c r="AL38" s="7"/>
+      <c r="AM38" s="7"/>
     </row>
     <row r="39" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
@@ -2168,25 +2175,27 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-      <c r="X39" s="1"/>
-      <c r="Y39" s="1"/>
-      <c r="Z39" s="1"/>
-      <c r="AA39" s="1"/>
-      <c r="AB39" s="1"/>
-      <c r="AC39" s="1"/>
-      <c r="AD39" s="1"/>
-      <c r="AE39" s="1"/>
-      <c r="AF39" s="1"/>
-      <c r="AG39" s="1"/>
-      <c r="AH39" s="1"/>
-      <c r="AI39" s="1"/>
-      <c r="AJ39" s="1"/>
-      <c r="AK39" s="1"/>
-      <c r="AL39" s="1"/>
-      <c r="AM39" s="1"/>
+      <c r="U39" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="11"/>
+      <c r="AC39" s="11"/>
+      <c r="AD39" s="11"/>
+      <c r="AE39" s="11"/>
+      <c r="AF39" s="11"/>
+      <c r="AG39" s="11"/>
+      <c r="AH39" s="11"/>
+      <c r="AI39" s="11"/>
+      <c r="AJ39" s="11"/>
+      <c r="AK39" s="11"/>
+      <c r="AL39" s="11"/>
+      <c r="AM39" s="11"/>
     </row>
     <row r="40" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
@@ -2309,9 +2318,7 @@
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
       <c r="AL42" s="1"/>
-      <c r="AM42" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="AM42" s="1"/>
     </row>
     <row r="43" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
@@ -2334,25 +2341,27 @@
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
-      <c r="U43" s="11"/>
-      <c r="V43" s="12"/>
-      <c r="W43" s="12"/>
-      <c r="X43" s="12"/>
-      <c r="Y43" s="12"/>
-      <c r="Z43" s="12"/>
-      <c r="AA43" s="12"/>
-      <c r="AB43" s="12"/>
-      <c r="AC43" s="12"/>
-      <c r="AD43" s="12"/>
-      <c r="AE43" s="12"/>
-      <c r="AF43" s="12"/>
-      <c r="AG43" s="12"/>
-      <c r="AH43" s="12"/>
-      <c r="AI43" s="12"/>
-      <c r="AJ43" s="12"/>
-      <c r="AK43" s="12"/>
-      <c r="AL43" s="12"/>
-      <c r="AM43" s="12"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1"/>
+      <c r="AB43" s="1"/>
+      <c r="AC43" s="1"/>
+      <c r="AD43" s="1"/>
+      <c r="AE43" s="1"/>
+      <c r="AF43" s="1"/>
+      <c r="AG43" s="1"/>
+      <c r="AH43" s="1"/>
+      <c r="AI43" s="1"/>
+      <c r="AJ43" s="1"/>
+      <c r="AK43" s="1"/>
+      <c r="AL43" s="1"/>
+      <c r="AM43" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="44" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
@@ -2375,27 +2384,25 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
-      <c r="U44" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="15"/>
-      <c r="AA44" s="15"/>
-      <c r="AB44" s="15"/>
-      <c r="AC44" s="15"/>
-      <c r="AD44" s="15"/>
-      <c r="AE44" s="15"/>
-      <c r="AF44" s="15"/>
-      <c r="AG44" s="15"/>
-      <c r="AH44" s="15"/>
-      <c r="AI44" s="15"/>
-      <c r="AJ44" s="15"/>
-      <c r="AK44" s="15"/>
-      <c r="AL44" s="15"/>
-      <c r="AM44" s="15"/>
+      <c r="U44" s="6"/>
+      <c r="V44" s="7"/>
+      <c r="W44" s="7"/>
+      <c r="X44" s="7"/>
+      <c r="Y44" s="7"/>
+      <c r="Z44" s="7"/>
+      <c r="AA44" s="7"/>
+      <c r="AB44" s="7"/>
+      <c r="AC44" s="7"/>
+      <c r="AD44" s="7"/>
+      <c r="AE44" s="7"/>
+      <c r="AF44" s="7"/>
+      <c r="AG44" s="7"/>
+      <c r="AH44" s="7"/>
+      <c r="AI44" s="7"/>
+      <c r="AJ44" s="7"/>
+      <c r="AK44" s="7"/>
+      <c r="AL44" s="7"/>
+      <c r="AM44" s="7"/>
     </row>
     <row r="45" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
@@ -2418,25 +2425,27 @@
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
-      <c r="U45" s="1"/>
-      <c r="V45" s="1"/>
-      <c r="W45" s="1"/>
-      <c r="X45" s="1"/>
-      <c r="Y45" s="1"/>
-      <c r="Z45" s="1"/>
-      <c r="AA45" s="1"/>
-      <c r="AB45" s="1"/>
-      <c r="AC45" s="1"/>
-      <c r="AD45" s="1"/>
-      <c r="AE45" s="1"/>
-      <c r="AF45" s="1"/>
-      <c r="AG45" s="1"/>
-      <c r="AH45" s="1"/>
-      <c r="AI45" s="1"/>
-      <c r="AJ45" s="1"/>
-      <c r="AK45" s="1"/>
-      <c r="AL45" s="1"/>
-      <c r="AM45" s="1"/>
+      <c r="U45" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11"/>
+      <c r="Y45" s="11"/>
+      <c r="Z45" s="11"/>
+      <c r="AA45" s="11"/>
+      <c r="AB45" s="11"/>
+      <c r="AC45" s="11"/>
+      <c r="AD45" s="11"/>
+      <c r="AE45" s="11"/>
+      <c r="AF45" s="11"/>
+      <c r="AG45" s="11"/>
+      <c r="AH45" s="11"/>
+      <c r="AI45" s="11"/>
+      <c r="AJ45" s="11"/>
+      <c r="AK45" s="11"/>
+      <c r="AL45" s="11"/>
+      <c r="AM45" s="11"/>
     </row>
     <row r="46" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
@@ -41593,29 +41602,70 @@
       <c r="AL1000" s="1"/>
       <c r="AM1000" s="1"/>
     </row>
+    <row r="1001" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="1"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="1"/>
+      <c r="G1001" s="1"/>
+      <c r="H1001" s="1"/>
+      <c r="I1001" s="1"/>
+      <c r="J1001" s="1"/>
+      <c r="K1001" s="1"/>
+      <c r="L1001" s="1"/>
+      <c r="M1001" s="1"/>
+      <c r="N1001" s="1"/>
+      <c r="O1001" s="1"/>
+      <c r="P1001" s="1"/>
+      <c r="Q1001" s="1"/>
+      <c r="R1001" s="1"/>
+      <c r="S1001" s="1"/>
+      <c r="T1001" s="1"/>
+      <c r="U1001" s="1"/>
+      <c r="V1001" s="1"/>
+      <c r="W1001" s="1"/>
+      <c r="X1001" s="1"/>
+      <c r="Y1001" s="1"/>
+      <c r="Z1001" s="1"/>
+      <c r="AA1001" s="1"/>
+      <c r="AB1001" s="1"/>
+      <c r="AC1001" s="1"/>
+      <c r="AD1001" s="1"/>
+      <c r="AE1001" s="1"/>
+      <c r="AF1001" s="1"/>
+      <c r="AG1001" s="1"/>
+      <c r="AH1001" s="1"/>
+      <c r="AI1001" s="1"/>
+      <c r="AJ1001" s="1"/>
+      <c r="AK1001" s="1"/>
+      <c r="AL1001" s="1"/>
+      <c r="AM1001" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="U43:AM43"/>
-    <mergeCell ref="A8:AM18"/>
-    <mergeCell ref="U44:AM44"/>
-    <mergeCell ref="Z27:AD27"/>
-    <mergeCell ref="AH27:AM27"/>
-    <mergeCell ref="AE27:AG27"/>
-    <mergeCell ref="AH29:AM29"/>
-    <mergeCell ref="AH30:AM30"/>
-    <mergeCell ref="U37:AM37"/>
-    <mergeCell ref="U38:AM38"/>
-    <mergeCell ref="AH28:AM28"/>
-    <mergeCell ref="Z28:AD28"/>
-    <mergeCell ref="AE28:AG28"/>
-    <mergeCell ref="A29:AG29"/>
-    <mergeCell ref="A30:AG30"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A21:AM25"/>
+    <mergeCell ref="A22:AM26"/>
+    <mergeCell ref="D29:V29"/>
+    <mergeCell ref="W29:Y29"/>
     <mergeCell ref="D28:V28"/>
     <mergeCell ref="W28:Y28"/>
-    <mergeCell ref="D27:V27"/>
-    <mergeCell ref="W27:Y27"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="U44:AM44"/>
+    <mergeCell ref="A9:AM19"/>
+    <mergeCell ref="U45:AM45"/>
+    <mergeCell ref="Z28:AD28"/>
+    <mergeCell ref="AH28:AM28"/>
+    <mergeCell ref="AE28:AG28"/>
+    <mergeCell ref="AH30:AM30"/>
+    <mergeCell ref="AH31:AM31"/>
+    <mergeCell ref="U38:AM38"/>
+    <mergeCell ref="U39:AM39"/>
+    <mergeCell ref="AH29:AM29"/>
+    <mergeCell ref="Z29:AD29"/>
+    <mergeCell ref="AE29:AG29"/>
+    <mergeCell ref="A30:AG30"/>
+    <mergeCell ref="A31:AG31"/>
     <mergeCell ref="A28:C28"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>